<commit_message>
-Added reliability measures. Needs interpretation.
</commit_message>
<xml_diff>
--- a/Data analytics/Language tests/Data/one_test_dichotomous_analysis_NRT.xlsx
+++ b/Data analytics/Language tests/Data/one_test_dichotomous_analysis_NRT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="89">
   <si>
     <t>Student</t>
   </si>
@@ -272,6 +272,15 @@
   </si>
   <si>
     <t>[35.0, 40.0, 50.0]</t>
+  </si>
+  <si>
+    <t>Reliability</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>SEM</t>
   </si>
 </sst>
 </file>
@@ -348,15 +357,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>125689</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>24825</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -374,7 +383,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4267200" y="9144000"/>
+          <a:off x="5486400" y="8191500"/>
           <a:ext cx="10488889" cy="4596825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3643,7 +3652,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
         <v>63</v>
       </c>
@@ -3659,8 +3668,14 @@
       <c r="E49" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="G49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
         <v>64</v>
       </c>
@@ -3676,8 +3691,14 @@
       <c r="E50">
         <v>49.9</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="G50" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H50">
+        <v>0.6751455645621645</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>65</v>
       </c>
@@ -3687,8 +3708,14 @@
       <c r="C51" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="G51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H51">
+        <v>2.039593469411941</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>66</v>
       </c>
@@ -3699,7 +3726,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>67</v>
       </c>
@@ -3710,7 +3737,7 @@
         <v>55.00000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
         <v>68</v>
       </c>
@@ -3721,7 +3748,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
         <v>69</v>
       </c>
@@ -3732,7 +3759,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
         <v>70</v>
       </c>
@@ -3743,7 +3770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
         <v>71</v>
       </c>
@@ -3754,7 +3781,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
         <v>72</v>
       </c>
@@ -3771,7 +3798,7 @@
         <v>9.984</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
         <v>73</v>
       </c>
@@ -3782,7 +3809,7 @@
         <v>18.19830104486516</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
         <v>74</v>
       </c>
@@ -3793,7 +3820,7 @@
         <v>3.20138888888889</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
         <v>75</v>
       </c>
@@ -3804,7 +3831,7 @@
         <v>3.311781609195403</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
         <v>76</v>
       </c>
@@ -3815,7 +3842,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
         <v>77</v>
       </c>
@@ -3826,7 +3853,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
-Applied Spearman-Brown prophecy formula to calculate a new length for the test.
</commit_message>
<xml_diff>
--- a/Data analytics/Language tests/Data/one_test_dichotomous_analysis_NRT.xlsx
+++ b/Data analytics/Language tests/Data/one_test_dichotomous_analysis_NRT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="92">
   <si>
     <t>Student</t>
   </si>
@@ -281,6 +281,15 @@
   </si>
   <si>
     <t>SEM</t>
+  </si>
+  <si>
+    <t>Reliable?</t>
+  </si>
+  <si>
+    <t>New No of Items</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -3695,7 +3704,7 @@
         <v>87</v>
       </c>
       <c r="H50">
-        <v>0.6751455645621645</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -3712,7 +3721,7 @@
         <v>88</v>
       </c>
       <c r="H51">
-        <v>2.039593469411941</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -3725,6 +3734,12 @@
       <c r="C52">
         <v>40</v>
       </c>
+      <c r="G52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H52" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
@@ -3735,6 +3750,12 @@
       </c>
       <c r="C53">
         <v>55.00000000000001</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H53">
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:8">

</xml_diff>